<commit_message>
UPDATE LESSON PLAN TEMPLATE
</commit_message>
<xml_diff>
--- a/content/post/2020-06-29-teaching-a-2-days-forecasting-in-r-workshop-virtually/priority.xlsx
+++ b/content/post/2020-06-29-teaching-a-2-days-forecasting-in-r-workshop-virtually/priority.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Documents/BRTBlog/content/post/2020-06-29-teaching-a-2-days-forecasting-in-r-workshop-virtually/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Documents/1.BRTBlog/content/post/2020-06-29-teaching-a-2-days-forecasting-in-r-workshop-virtually/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BAC0F-7E9E-9440-8C57-2169AF6C638C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44CFC43-25E9-324F-85F1-0F0C2D66836E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{1532A227-53F9-A947-ABAE-BFD2B9CD8349}"/>
   </bookViews>
@@ -287,19 +287,19 @@
     <t>What is the current level of skills and knowledge of learners?(3,2,1,0)</t>
   </si>
   <si>
-    <t>How important is the task to the task(main steps  of the forecasting process) ? (3,2,1,0)</t>
-  </si>
-  <si>
     <t>use it few times</t>
   </si>
   <si>
-    <t>time allocated(min)</t>
-  </si>
-  <si>
     <t>cumulative time</t>
   </si>
   <si>
     <t>ETS framework</t>
+  </si>
+  <si>
+    <t>How important is the task to the learning outcome of the topic ? (3,2,1,0)</t>
+  </si>
+  <si>
+    <t>allocated time (min)</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2194E4D-DFDA-F94F-9EBC-5DD647DDEBC4}">
   <dimension ref="B2:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
@@ -786,10 +786,10 @@
         <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>27</v>
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="8">
-        <f>SUM(D3:G3)</f>
+        <f t="shared" ref="H3:H13" si="0">SUM(D3:G3)</f>
         <v>12</v>
       </c>
       <c r="I3" s="8">
@@ -826,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="K3" s="6" t="str">
-        <f>IF(H3&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" ref="K3:K13" si="1">IF(H3&lt;= 6, "Good to Know","Must to Know")</f>
         <v>Must to Know</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="6">
-        <f>SUM(D4:G4)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I4" s="6">
@@ -861,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="K4" s="6" t="str">
-        <f>IF(H4&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -885,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="8">
-        <f>SUM(D5:G5)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I5" s="8">
@@ -896,7 +896,7 @@
         <v>24</v>
       </c>
       <c r="K5" s="6" t="str">
-        <f>IF(H5&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="8">
-        <f>SUM(D6:G6)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I6" s="8">
@@ -931,7 +931,7 @@
         <v>31</v>
       </c>
       <c r="K6" s="6" t="str">
-        <f>IF(H6&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -955,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="8">
-        <f>SUM(D7:G7)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I7" s="8">
@@ -966,7 +966,7 @@
         <v>38</v>
       </c>
       <c r="K7" s="6" t="str">
-        <f>IF(H7&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -990,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="8">
-        <f>SUM(D8:G8)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I8" s="8">
@@ -1001,7 +1001,7 @@
         <v>45</v>
       </c>
       <c r="K8" s="6" t="str">
-        <f>IF(H8&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -1025,18 +1025,18 @@
         <v>2</v>
       </c>
       <c r="H9" s="8">
-        <f>SUM(D9:G9)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I9" s="8">
         <v>7</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" ref="J9:J13" si="0">J8+I9</f>
+        <f t="shared" ref="J9:J13" si="2">J8+I9</f>
         <v>52</v>
       </c>
       <c r="K9" s="6" t="str">
-        <f>IF(H9&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -1060,18 +1060,18 @@
         <v>2</v>
       </c>
       <c r="H10" s="8">
-        <f>SUM(D10:G10)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I10" s="8">
         <v>7</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="K10" s="6" t="str">
-        <f>IF(H10&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Must to Know</v>
       </c>
     </row>
@@ -1095,18 +1095,18 @@
         <v>0</v>
       </c>
       <c r="H11" s="9">
-        <f>SUM(D11:G11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I11" s="9">
         <v>7</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="K11" s="9" t="str">
-        <f>IF(H11&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Good to Know</v>
       </c>
     </row>
@@ -1130,18 +1130,18 @@
         <v>0</v>
       </c>
       <c r="H12" s="9">
-        <f>SUM(D12:G12)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I12" s="9">
         <v>7</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="K12" s="9" t="str">
-        <f>IF(H12&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Good to Know</v>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="13">
         <v>2</v>
@@ -1165,18 +1165,18 @@
         <v>0</v>
       </c>
       <c r="H13" s="9">
-        <f>SUM(D13:G13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I13" s="9">
         <v>7</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="K13" s="9" t="str">
-        <f>IF(H13&lt;= 6, "Good to Know","Must to Know")</f>
+        <f t="shared" si="1"/>
         <v>Good to Know</v>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>31</v>

</xml_diff>